<commit_message>
Added new classes and functions to support FEMS Contracts (Operations) such as OperationalCFs and Investments
</commit_message>
<xml_diff>
--- a/src/data/bankA/Operations.xlsx
+++ b/src/data/bankA/Operations.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/viganhamzai/Documents/ZHAW_WI/07_Semester/PA/PA_FEMS/src/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/viganhamzai/Documents/ZHAW_WI/07_Semester/PA/PA_FEMS/src/data/bankA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB3E77C8-25DB-2A47-82B2-AB33C88CCE2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{661CE686-B252-DB41-A35F-A475777F7059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="2000" windowWidth="27640" windowHeight="16940" xr2:uid="{6112ACC4-624F-E94D-BE34-4C26021859BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,26 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="33">
-  <si>
-    <t>ContractType</t>
-  </si>
-  <si>
-    <t>ContractID</t>
-  </si>
-  <si>
-    <t>Currency</t>
-  </si>
-  <si>
-    <t>amount</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="35">
   <si>
     <t>repetition</t>
   </si>
   <si>
-    <t>startDate</t>
-  </si>
-  <si>
     <t>frequency</t>
   </si>
   <si>
@@ -65,9 +50,6 @@
     <t>description</t>
   </si>
   <si>
-    <t>Investment</t>
-  </si>
-  <si>
     <t>AFA0001</t>
   </si>
   <si>
@@ -135,12 +117,39 @@
   </si>
   <si>
     <t>Yearly rent expenses</t>
+  </si>
+  <si>
+    <t>Investments</t>
+  </si>
+  <si>
+    <t>initialExchangeDate</t>
+  </si>
+  <si>
+    <t>maturityDate</t>
+  </si>
+  <si>
+    <t>notionalPrincipal</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>contractID</t>
+  </si>
+  <si>
+    <t>contractType</t>
+  </si>
+  <si>
+    <t>inverted</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -172,7 +181,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -487,332 +496,400 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DD39D0B-D0CF-AD4D-84ED-3FA26222419A}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="54.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5" customWidth="1"/>
+    <col min="7" max="8" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="54.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="H1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="I1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="J1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D2">
         <v>8500000</v>
       </c>
+      <c r="E2" s="1">
+        <v>44562</v>
+      </c>
       <c r="F2" s="1">
-        <v>44562</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2">
+        <v>2958101</v>
+      </c>
+      <c r="H2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2">
         <v>51</v>
       </c>
-      <c r="I2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <v>3500000</v>
       </c>
+      <c r="E3" s="1">
+        <v>44562</v>
+      </c>
       <c r="F3" s="1">
-        <v>44562</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3">
+        <v>2958101</v>
+      </c>
+      <c r="H3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3">
         <v>51</v>
       </c>
-      <c r="I3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D4">
         <v>6000000</v>
       </c>
+      <c r="E4" s="1">
+        <v>44562</v>
+      </c>
       <c r="F4" s="1">
-        <v>44562</v>
-      </c>
-      <c r="G4" t="s">
+        <v>2958101</v>
+      </c>
+      <c r="H4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4">
+        <v>51</v>
+      </c>
+      <c r="J4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="H4">
-        <v>51</v>
-      </c>
-      <c r="I4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D5">
         <v>2000000</v>
       </c>
+      <c r="E5" s="1">
+        <v>44562</v>
+      </c>
       <c r="F5" s="1">
-        <v>44562</v>
-      </c>
-      <c r="G5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5">
+        <v>2958101</v>
+      </c>
+      <c r="H5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5">
         <v>11</v>
       </c>
-      <c r="I5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D6">
         <v>1000000</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
+        <v>44562</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2958101</v>
+      </c>
+      <c r="G6">
         <v>10</v>
       </c>
-      <c r="F6" s="1">
-        <v>44562</v>
-      </c>
-      <c r="G6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6">
+      <c r="H6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6">
         <v>11</v>
       </c>
-      <c r="I6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J6" t="b">
+        <v>0</v>
+      </c>
+      <c r="K6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D7">
         <f>0.05*D2</f>
         <v>425000</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
+        <v>44562</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2958101</v>
+      </c>
+      <c r="G7">
         <v>50</v>
       </c>
-      <c r="F7" s="1">
-        <v>44562</v>
-      </c>
-      <c r="G7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7">
+      <c r="H7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7">
         <v>51</v>
       </c>
-      <c r="I7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J7" t="b">
+        <v>1</v>
+      </c>
+      <c r="K7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D8">
         <f>0.05*D3</f>
         <v>175000</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="1">
+        <v>44562</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2958101</v>
+      </c>
+      <c r="G8">
         <v>50</v>
       </c>
-      <c r="F8" s="1">
-        <v>44562</v>
-      </c>
-      <c r="G8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8">
+      <c r="H8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8">
         <v>51</v>
       </c>
-      <c r="I8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D9">
         <f>0.05*D4</f>
         <v>300000</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
+        <v>44562</v>
+      </c>
+      <c r="F9" s="1">
+        <v>2958101</v>
+      </c>
+      <c r="G9">
         <v>50</v>
       </c>
-      <c r="F9" s="1">
-        <v>44562</v>
-      </c>
-      <c r="G9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9">
+      <c r="H9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9">
         <v>51</v>
       </c>
-      <c r="I9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J9" t="b">
+        <v>1</v>
+      </c>
+      <c r="K9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D10">
         <v>2000000</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="1">
+        <v>44562</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2958101</v>
+      </c>
+      <c r="G10">
         <v>10</v>
       </c>
-      <c r="F10" s="1">
-        <v>44562</v>
-      </c>
-      <c r="G10" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10">
+      <c r="H10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10">
         <v>11</v>
       </c>
-      <c r="I10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J10" t="b">
+        <v>0</v>
+      </c>
+      <c r="K10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D11">
         <v>1200000</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="1">
+        <v>44562</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2958101</v>
+      </c>
+      <c r="G11">
         <v>10</v>
       </c>
-      <c r="F11" s="1">
-        <v>44562</v>
-      </c>
-      <c r="G11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11">
+      <c r="H11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11">
         <v>11</v>
       </c>
-      <c r="I11" t="s">
-        <v>32</v>
+      <c r="J11" t="b">
+        <v>0</v>
+      </c>
+      <c r="K11" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adjust expense Operations to be negative
</commit_message>
<xml_diff>
--- a/src/data/bankA/Operations.xlsx
+++ b/src/data/bankA/Operations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/viganhamzai/Documents/ZHAW_WI/07_Semester/PA/PA_FEMS/src/data/bankA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{661CE686-B252-DB41-A35F-A475777F7059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E0A2E4-F863-5247-9536-2E435278BD1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="2000" windowWidth="27640" windowHeight="16940" xr2:uid="{6112ACC4-624F-E94D-BE34-4C26021859BF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="38">
   <si>
     <t>repetition</t>
   </si>
@@ -141,6 +141,15 @@
   </si>
   <si>
     <t>inverted</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>short</t>
   </si>
 </sst>
 </file>
@@ -148,7 +157,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -181,7 +190,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -496,27 +505,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DD39D0B-D0CF-AD4D-84ED-3FA26222419A}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5" customWidth="1"/>
-    <col min="7" max="8" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="54.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5" customWidth="1"/>
+    <col min="8" max="9" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="54.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -524,34 +534,37 @@
         <v>32</v>
       </c>
       <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
         <v>31</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>30</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>28</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>29</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>0</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>1</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>2</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>34</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -559,31 +572,34 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>8500000</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
         <v>44562</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>2958101</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>6</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>51</v>
       </c>
-      <c r="J2" t="b">
+      <c r="K2" t="b">
         <v>0</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -591,31 +607,34 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" t="s">
         <v>5</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>3500000</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F3" s="1">
         <v>44562</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="1">
         <v>2958101</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>6</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>51</v>
       </c>
-      <c r="J3" t="b">
+      <c r="K3" t="b">
         <v>0</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -623,31 +642,34 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" t="s">
         <v>5</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>6000000</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4" s="1">
         <v>44562</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="1">
         <v>2958101</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>6</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>51</v>
       </c>
-      <c r="J4" t="b">
+      <c r="K4" t="b">
         <v>0</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -655,31 +677,34 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" t="s">
         <v>5</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>2000000</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F5" s="1">
         <v>44562</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G5" s="1">
         <v>2958101</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>6</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>11</v>
       </c>
-      <c r="J5" t="b">
+      <c r="K5" t="b">
         <v>0</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -687,34 +712,37 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" t="s">
         <v>5</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>1000000</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="1">
         <v>44562</v>
       </c>
-      <c r="F6" s="1">
+      <c r="G6" s="1">
         <v>2958101</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>10</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>6</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>11</v>
       </c>
-      <c r="J6" t="b">
+      <c r="K6" t="b">
         <v>0</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -722,35 +750,38 @@
         <v>17</v>
       </c>
       <c r="C7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" t="s">
         <v>5</v>
       </c>
-      <c r="D7">
-        <f>0.05*D2</f>
+      <c r="E7">
+        <f>0.05*E2</f>
         <v>425000</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7" s="1">
         <v>44562</v>
       </c>
-      <c r="F7" s="1">
+      <c r="G7" s="1">
         <v>2958101</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>50</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>6</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>51</v>
       </c>
-      <c r="J7" t="b">
+      <c r="K7" t="b">
         <v>1</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -758,35 +789,38 @@
         <v>19</v>
       </c>
       <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" t="s">
         <v>5</v>
       </c>
-      <c r="D8">
-        <f>0.05*D3</f>
+      <c r="E8">
+        <f>0.05*E3</f>
         <v>175000</v>
       </c>
-      <c r="E8" s="1">
+      <c r="F8" s="1">
         <v>44562</v>
       </c>
-      <c r="F8" s="1">
+      <c r="G8" s="1">
         <v>2958101</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>50</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>6</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>51</v>
       </c>
-      <c r="J8" t="b">
+      <c r="K8" t="b">
         <v>1</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -794,35 +828,38 @@
         <v>21</v>
       </c>
       <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" t="s">
         <v>5</v>
       </c>
-      <c r="D9">
-        <f>0.05*D4</f>
+      <c r="E9">
+        <f>0.05*E4</f>
         <v>300000</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F9" s="1">
         <v>44562</v>
       </c>
-      <c r="F9" s="1">
+      <c r="G9" s="1">
         <v>2958101</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>50</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>6</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>51</v>
       </c>
-      <c r="J9" t="b">
+      <c r="K9" t="b">
         <v>1</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -830,34 +867,37 @@
         <v>23</v>
       </c>
       <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" t="s">
         <v>5</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>2000000</v>
       </c>
-      <c r="E10" s="1">
+      <c r="F10" s="1">
         <v>44562</v>
       </c>
-      <c r="F10" s="1">
+      <c r="G10" s="1">
         <v>2958101</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>10</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>6</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>11</v>
       </c>
-      <c r="J10" t="b">
+      <c r="K10" t="b">
         <v>0</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -865,30 +905,33 @@
         <v>25</v>
       </c>
       <c r="C11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" t="s">
         <v>5</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>1200000</v>
       </c>
-      <c r="E11" s="1">
+      <c r="F11" s="1">
         <v>44562</v>
       </c>
-      <c r="F11" s="1">
+      <c r="G11" s="1">
         <v>2958101</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>10</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>6</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>11</v>
       </c>
-      <c r="J11" t="b">
+      <c r="K11" t="b">
         <v>0</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change opreations attribute from role to contractRole
</commit_message>
<xml_diff>
--- a/src/data/bankA/Operations.xlsx
+++ b/src/data/bankA/Operations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/viganhamzai/Documents/ZHAW_WI/07_Semester/PA/PA_FEMS/src/data/bankA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E0A2E4-F863-5247-9536-2E435278BD1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A8A2AC-A3F2-DE43-9B7E-925CCF5BC5C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="2000" windowWidth="27640" windowHeight="16940" xr2:uid="{6112ACC4-624F-E94D-BE34-4C26021859BF}"/>
   </bookViews>
@@ -143,13 +143,13 @@
     <t>inverted</t>
   </si>
   <si>
-    <t>role</t>
-  </si>
-  <si>
     <t>long</t>
   </si>
   <si>
     <t>short</t>
+  </si>
+  <si>
+    <t>contractRole</t>
   </si>
 </sst>
 </file>
@@ -508,14 +508,14 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
@@ -534,7 +534,7 @@
         <v>32</v>
       </c>
       <c r="C1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D1" t="s">
         <v>31</v>
@@ -572,7 +572,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
@@ -607,7 +607,7 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -642,7 +642,7 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
@@ -677,7 +677,7 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
@@ -712,7 +712,7 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
@@ -750,7 +750,7 @@
         <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
@@ -789,7 +789,7 @@
         <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D8" t="s">
         <v>5</v>
@@ -828,7 +828,7 @@
         <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
         <v>5</v>
@@ -867,7 +867,7 @@
         <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10" t="s">
         <v>5</v>
@@ -905,7 +905,7 @@
         <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
         <v>5</v>

</xml_diff>